<commit_message>
Export von Zerfallskorrektur nach Excel
https://terrapi.goip.de/b/XhP3cNp7GCAjvL2hS/programme/D8ERWcDrv8oWwSWhw
</commit_message>
<xml_diff>
--- a/src/Parameter.xlsx
+++ b/src/Parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Projekte\NuVe\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54FDF63-E5AB-4A10-A992-819D283099D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9F854-69E3-4683-95CF-0107EC018D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="816" windowWidth="12960" windowHeight="10560" tabRatio="752" firstSheet="3" activeTab="4" xr2:uid="{A72651EC-7529-46AF-A0BF-E1ABAC97BDF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="752" activeTab="3" xr2:uid="{A72651EC-7529-46AF-A0BF-E1ABAC97BDF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Eingabe" sheetId="2" r:id="rId1"/>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839BFC99-308E-42E9-9504-8CC5382CFD48}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2878,9 +2878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A4A71E-AA3F-4057-ABDF-8BD7DFD70944}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4291,7 +4291,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1">
         <v>0.3</v>
@@ -4321,7 +4321,7 @@
         <v>3</v>
       </c>
       <c r="M32" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N32" s="1">
         <v>0.4</v>
@@ -4336,7 +4336,7 @@
         <v>100</v>
       </c>
       <c r="C33" s="1">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1">
         <v>10</v>
@@ -4366,7 +4366,7 @@
         <v>80</v>
       </c>
       <c r="M33" s="1">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="N33" s="1">
         <v>80</v>
@@ -4382,7 +4382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F37F890-777E-4BC5-8682-71DF69E700E3}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -5132,7 +5132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B2BD30-B8F8-4DCB-A090-656B4B329DB3}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>